<commit_message>
Added seasonal statistics and a combined RSTs value sheet (done in a very ugly way, refactor later)
</commit_message>
<xml_diff>
--- a/python/Statistics/Results/Results for 00Z/classification_comparison_00Z_1979-2016.xlsx
+++ b/python/Statistics/Results/Results for 00Z/classification_comparison_00Z_1979-2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hatzv\Documents\Geography\RSTs\python\Statistics\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hatzv\Documents\Geography\RSTs\python\Statistics\Results\Results for 00Z\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t>1979-2016</t>
-  </si>
-  <si>
     <t>RST East</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>ERA 2.5 -Central</t>
+  </si>
+  <si>
+    <t>1979-2016 00Z</t>
   </si>
 </sst>
 </file>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,69 +505,69 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>1418</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>47</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>84</v>
@@ -808,13 +808,13 @@
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="U6">
-        <f>SUM(U2:U5)</f>
-        <v>13880</v>
+        <f>SUM(U3:U5)</f>
+        <v>1340</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>1565</v>
@@ -873,10 +873,14 @@
       <c r="T7">
         <v>87</v>
       </c>
+      <c r="U7">
+        <f>SUM(B7:T7)</f>
+        <v>12933</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -919,6 +923,10 @@
       </c>
       <c r="R8">
         <v>19</v>
+      </c>
+      <c r="U8">
+        <f>SUM(B8:T8)</f>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -976,10 +984,14 @@
       <c r="T9">
         <v>5</v>
       </c>
+      <c r="U9">
+        <f>SUM(B9:T9)</f>
+        <v>544</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>23</v>
@@ -1020,13 +1032,21 @@
       <c r="T10">
         <v>5</v>
       </c>
+      <c r="U10">
+        <f>SUM(B10:T10)</f>
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
+      <c r="U11">
+        <f>SUM(U8:U10)</f>
+        <v>947</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>1279</v>
@@ -1085,10 +1105,14 @@
       <c r="T12">
         <v>86</v>
       </c>
+      <c r="U12">
+        <f>SUM(B12:T12)</f>
+        <v>12100</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>209</v>
@@ -1140,6 +1164,10 @@
       </c>
       <c r="S13">
         <v>6</v>
+      </c>
+      <c r="U13">
+        <f>SUM(B13:T13)</f>
+        <v>533</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1203,10 +1231,14 @@
       <c r="T14">
         <v>6</v>
       </c>
+      <c r="U14">
+        <f>SUM(B14:T14)</f>
+        <v>803</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>95</v>
@@ -1255,6 +1287,16 @@
       </c>
       <c r="T15">
         <v>5</v>
+      </c>
+      <c r="U15">
+        <f>SUM(B15:T15)</f>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <f>SUM(U13:U15)</f>
+        <v>1780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>